<commit_message>
tbsp bacfill from rates diff
</commit_message>
<xml_diff>
--- a/julia_msp/assets_data_03.24.xlsx
+++ b/julia_msp/assets_data_03.24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matsz\programowanie\Optymalizacja_portfela\julia_msp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C2964F65-AC82-4FBA-B9A3-5534075D0D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4BAFC970-DDB6-4566-BEAC-48FB20E4E251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{829AE8ED-45E1-4F31-B65E-E75D41917891}"/>
   </bookViews>
@@ -1029,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A25BAC-A915-40C4-887C-670A87583871}">
   <dimension ref="A1:I617"/>
   <sheetViews>
-    <sheetView topLeftCell="A601" workbookViewId="0">
-      <selection activeCell="H618" sqref="H618"/>
+    <sheetView topLeftCell="A355" workbookViewId="0">
+      <selection activeCell="H363" sqref="H363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12133,8 +12133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B758B9-60FA-43E4-B0DC-3A660011F3DB}">
   <dimension ref="A1:K616"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A353" workbookViewId="0">
-      <selection activeCell="K616" sqref="K362:K616"/>
+    <sheetView tabSelected="1" topLeftCell="A349" workbookViewId="0">
+      <selection activeCell="J362" sqref="J362:K362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15985,14 +15985,6 @@
       <c r="I362">
         <f>Indexes!I363/12</f>
         <v>4.7783333333333332E-3</v>
-      </c>
-      <c r="J362">
-        <f>Indexes!H363-Indexes!H362</f>
-        <v>6.4699999999999994E-2</v>
-      </c>
-      <c r="K362">
-        <f>Indexes!I363-Indexes!I362</f>
-        <v>5.7340000000000002E-2</v>
       </c>
     </row>
     <row r="363" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>